<commit_message>
sales analysis report final version
</commit_message>
<xml_diff>
--- a/PowerBI_dashboards/PB_sales_analysis/Sales_report_seznam.xlsx
+++ b/PowerBI_dashboards/PB_sales_analysis/Sales_report_seznam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\portfolio\PowerBI_dashboards\PD_salesman_card\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\portfolio\PowerBI_dashboards\PB_sales_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61AF5B0-2888-4EC7-843B-A2B7CA2FBBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6F33B8-56B0-4ED7-BF3C-8BC6332F814B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Clients" sheetId="3" r:id="rId1"/>
@@ -4023,9 +4023,6 @@
     <t>Fraier</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=fRGaLMmzZJU</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=WxOiJKNKVYM</t>
   </si>
   <si>
@@ -4033,6 +4030,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=fRGaLMmzZJU&amp;t=946s</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -5878,45 +5878,40 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7B3AD2-AFC3-45F3-9AA7-FF3889906349}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1329</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
         <v>1330</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="G3" t="s">
         <v>1331</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{10420F93-95C4-4D45-B397-DCCD3AB44A50}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{A67B9EA9-BC0D-4AF1-860A-AEEFEE4AC632}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{AA49857D-FE81-4299-BC60-04F456B5763F}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{DB567C79-2230-4C15-B447-34744EA1F78E}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AA49857D-FE81-4299-BC60-04F456B5763F}"/>
+    <hyperlink ref="A1" r:id="rId2" xr:uid="{DB567C79-2230-4C15-B447-34744EA1F78E}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{0DA6A7FC-BB2F-4A97-826F-A62D73BCE3B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -83851,21 +83846,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010062A81288A2DF3744AFC9FA0F5812F5CA" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a60506152b6ca4a65ee667192a05dfe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eb266719-d799-4a2f-a400-35c1e34cc5b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fa2ab73d522e84d1e33bb5ab143c5e1" ns2:_="">
     <xsd:import namespace="eb266719-d799-4a2f-a400-35c1e34cc5b5"/>
@@ -83997,6 +83977,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{005B8A53-2C49-4728-A31E-9597C3B62963}">
   <ds:schemaRefs>
@@ -84006,23 +84001,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22927AFF-E3E8-40E0-985A-F23E77C72F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963C3BB3-AEC3-4F6B-B82F-6AD21CA407F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD5C287A-972A-4244-936E-523B8C5C0C7A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -84038,4 +84016,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{963C3BB3-AEC3-4F6B-B82F-6AD21CA407F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22927AFF-E3E8-40E0-985A-F23E77C72F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>